<commit_message>
Completed EnhancedALU.hdl, fixed bugs in EnhancedALU.cmp & EnhancedALU.xlsx.
</commit_message>
<xml_diff>
--- a/projects/05/EnhancedALU.xlsx
+++ b/projects/05/EnhancedALU.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="73">
   <si>
     <t>c1</t>
   </si>
@@ -246,13 +246,22 @@
   </si>
   <si>
     <t>OR</t>
+  </si>
+  <si>
+    <t>DC(=Don't care)</t>
+  </si>
+  <si>
+    <t>minusD</t>
+  </si>
+  <si>
+    <t>minusAM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,6 +279,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -484,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -560,21 +576,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -588,6 +589,59 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -897,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="C4:H4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,30 +967,30 @@
       <c r="A1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="K1" s="27" t="s">
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="K1" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
     </row>
     <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -956,16 +1010,16 @@
       <c r="L2" s="17"/>
       <c r="M2" s="17"/>
       <c r="N2" s="17"/>
-      <c r="O2" s="27" t="s">
+      <c r="O2" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="27"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
     </row>
     <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="13" t="s">
@@ -1063,7 +1117,7 @@
         <v>56</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="P4" s="11" t="s">
         <v>46</v>
@@ -1178,8 +1232,8 @@
       <c r="N6" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="O6" s="3" t="s">
-        <v>47</v>
+      <c r="O6" s="42" t="s">
+        <v>60</v>
       </c>
       <c r="P6" s="11" t="s">
         <v>46</v>
@@ -1187,8 +1241,8 @@
       <c r="Q6" s="4">
         <v>0</v>
       </c>
-      <c r="R6" s="4">
-        <v>1</v>
+      <c r="R6" s="41">
+        <v>0</v>
       </c>
       <c r="S6" s="4">
         <v>1</v>
@@ -1440,60 +1494,61 @@
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="4">
-        <v>0</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4">
-        <v>1</v>
-      </c>
-      <c r="F11" s="4">
-        <v>1</v>
-      </c>
-      <c r="G11" s="4">
-        <v>1</v>
-      </c>
-      <c r="H11" s="11">
-        <v>1</v>
-      </c>
-      <c r="I11" s="5"/>
-      <c r="K11" s="22" t="s">
+      <c r="C11" s="41">
+        <v>0</v>
+      </c>
+      <c r="D11" s="41">
+        <v>0</v>
+      </c>
+      <c r="E11" s="41">
+        <v>1</v>
+      </c>
+      <c r="F11" s="41">
+        <v>1</v>
+      </c>
+      <c r="G11" s="41">
+        <v>1</v>
+      </c>
+      <c r="H11" s="47">
+        <v>1</v>
+      </c>
+      <c r="I11" s="48"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="L11" s="17" t="s">
+      <c r="L11" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17" t="s">
+      <c r="M11" s="51"/>
+      <c r="N11" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="O11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P11" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q11" s="4">
-        <v>0</v>
-      </c>
-      <c r="R11" s="4">
-        <v>1</v>
-      </c>
-      <c r="S11" s="4">
-        <v>0</v>
-      </c>
-      <c r="T11" s="11">
-        <v>0</v>
-      </c>
-      <c r="U11" s="4">
-        <v>1</v>
-      </c>
-      <c r="V11" s="5">
+      <c r="O11" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="P11" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q11" s="41">
+        <v>0</v>
+      </c>
+      <c r="R11" s="41">
+        <v>0</v>
+      </c>
+      <c r="S11" s="41">
+        <v>1</v>
+      </c>
+      <c r="T11" s="47">
+        <v>0</v>
+      </c>
+      <c r="U11" s="41">
+        <v>1</v>
+      </c>
+      <c r="V11" s="48">
         <v>0</v>
       </c>
       <c r="W11" t="s">
@@ -1535,14 +1590,14 @@
       <c r="N12" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="O12" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="P12" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q12" s="4">
-        <v>0</v>
+      <c r="O12" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="P12" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q12" s="41">
+        <v>1</v>
       </c>
       <c r="R12" s="4">
         <v>0</v>
@@ -1550,8 +1605,8 @@
       <c r="S12" s="4">
         <v>0</v>
       </c>
-      <c r="T12" s="11">
-        <v>1</v>
+      <c r="T12" s="47">
+        <v>0</v>
       </c>
       <c r="U12" s="4">
         <v>1</v>
@@ -1596,10 +1651,10 @@
       <c r="O13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="P13" s="39" t="s">
+      <c r="P13" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="Q13" s="4">
+      <c r="Q13" s="41">
         <v>0</v>
       </c>
       <c r="R13" s="4">
@@ -1659,7 +1714,7 @@
       <c r="P14" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="Q14" s="4">
+      <c r="Q14" s="41">
         <v>0</v>
       </c>
       <c r="R14" s="4">
@@ -1714,10 +1769,10 @@
       <c r="O15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="P15" s="39" t="s">
+      <c r="P15" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="Q15" s="4">
+      <c r="Q15" s="41">
         <v>0</v>
       </c>
       <c r="R15" s="4">
@@ -1777,7 +1832,7 @@
       <c r="P16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="Q16" s="4">
+      <c r="Q16" s="41">
         <v>0</v>
       </c>
       <c r="R16" s="4">
@@ -1856,123 +1911,124 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="15" t="s">
+    <row r="18" spans="2:22" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="4">
-        <v>0</v>
-      </c>
-      <c r="D18" s="4">
-        <v>1</v>
-      </c>
-      <c r="E18" s="4">
-        <v>0</v>
-      </c>
-      <c r="F18" s="4">
-        <v>0</v>
-      </c>
-      <c r="G18" s="4">
-        <v>1</v>
-      </c>
-      <c r="H18" s="11">
-        <v>1</v>
-      </c>
-      <c r="I18" s="5" t="s">
+      <c r="C18" s="41">
+        <v>0</v>
+      </c>
+      <c r="D18" s="41">
+        <v>1</v>
+      </c>
+      <c r="E18" s="41">
+        <v>0</v>
+      </c>
+      <c r="F18" s="41">
+        <v>0</v>
+      </c>
+      <c r="G18" s="41">
+        <v>1</v>
+      </c>
+      <c r="H18" s="47">
+        <v>1</v>
+      </c>
+      <c r="I18" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="K18" s="22" t="s">
+      <c r="K18" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="L18" s="17" t="s">
+      <c r="L18" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17" t="s">
+      <c r="M18" s="45"/>
+      <c r="N18" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="O18" s="6" t="s">
+      <c r="O18" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="P18" s="11" t="s">
+      <c r="P18" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q18" s="41">
+        <v>0</v>
+      </c>
+      <c r="R18" s="41">
+        <v>0</v>
+      </c>
+      <c r="S18" s="41">
+        <v>0</v>
+      </c>
+      <c r="T18" s="47">
+        <v>1</v>
+      </c>
+      <c r="U18" s="41">
+        <v>1</v>
+      </c>
+      <c r="V18" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="41">
+        <v>0</v>
+      </c>
+      <c r="D19" s="41">
+        <v>0</v>
+      </c>
+      <c r="E19" s="41">
+        <v>0</v>
+      </c>
+      <c r="F19" s="41">
+        <v>1</v>
+      </c>
+      <c r="G19" s="41">
+        <v>1</v>
+      </c>
+      <c r="H19" s="47">
+        <v>1</v>
+      </c>
+      <c r="I19" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" s="43"/>
+      <c r="K19" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="L19" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="M19" s="45"/>
+      <c r="N19" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="O19" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="P19" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="Q18" s="4">
-        <v>0</v>
-      </c>
-      <c r="R18" s="4">
-        <v>0</v>
-      </c>
-      <c r="S18" s="4">
-        <v>0</v>
-      </c>
-      <c r="T18" s="11">
-        <v>1</v>
-      </c>
-      <c r="U18" s="4">
-        <v>1</v>
-      </c>
-      <c r="V18" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B19" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="4">
-        <v>0</v>
-      </c>
-      <c r="D19" s="4">
-        <v>0</v>
-      </c>
-      <c r="E19" s="4">
-        <v>0</v>
-      </c>
-      <c r="F19" s="4">
-        <v>1</v>
-      </c>
-      <c r="G19" s="4">
-        <v>1</v>
-      </c>
-      <c r="H19" s="11">
-        <v>1</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K19" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="L19" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="M19" s="17"/>
-      <c r="N19" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="O19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P19" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q19" s="4">
-        <v>0</v>
-      </c>
-      <c r="R19" s="4">
-        <v>1</v>
-      </c>
-      <c r="S19" s="4">
-        <v>0</v>
-      </c>
-      <c r="T19" s="11">
-        <v>0</v>
-      </c>
-      <c r="U19" s="4">
-        <v>1</v>
-      </c>
-      <c r="V19" s="5">
+      <c r="Q19" s="41">
+        <v>0</v>
+      </c>
+      <c r="R19" s="41">
+        <v>0</v>
+      </c>
+      <c r="S19" s="41">
+        <v>0</v>
+      </c>
+      <c r="T19" s="47">
+        <v>0</v>
+      </c>
+      <c r="U19" s="41">
+        <v>1</v>
+      </c>
+      <c r="V19" s="48">
         <v>0</v>
       </c>
     </row>
@@ -2071,7 +2127,7 @@
       <c r="N21" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="O21" s="40" t="s">
+      <c r="O21" s="35" t="s">
         <v>8</v>
       </c>
       <c r="P21" s="12" t="s">
@@ -2103,20 +2159,20 @@
       </c>
       <c r="C23" s="24"/>
       <c r="D23" s="24"/>
-      <c r="I23" s="28" t="s">
+      <c r="I23" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="29"/>
-      <c r="N23" s="29"/>
-      <c r="O23" s="30"/>
-      <c r="Q23" s="28" t="s">
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="39"/>
+      <c r="O23" s="40"/>
+      <c r="Q23" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="R23" s="29"/>
-      <c r="S23" s="30"/>
+      <c r="R23" s="39"/>
+      <c r="S23" s="40"/>
     </row>
     <row r="24" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="23" t="s">
@@ -2127,23 +2183,23 @@
       <c r="I24" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J24" s="37" t="s">
+      <c r="J24" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="K24" s="37"/>
-      <c r="L24" s="37"/>
-      <c r="M24" s="37"/>
-      <c r="N24" s="37"/>
-      <c r="O24" s="38" t="s">
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="33" t="s">
         <v>67</v>
       </c>
       <c r="Q24" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="R24" s="37" t="s">
+      <c r="R24" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="S24" s="38" t="s">
+      <c r="S24" s="33" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2153,26 +2209,26 @@
       </c>
       <c r="C25" s="24"/>
       <c r="D25" s="24"/>
-      <c r="I25" s="33">
-        <v>0</v>
-      </c>
-      <c r="J25" s="31">
-        <v>0</v>
-      </c>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="31"/>
-      <c r="O25" s="32">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="33">
-        <v>0</v>
-      </c>
-      <c r="R25" s="31">
-        <v>0</v>
-      </c>
-      <c r="S25" s="32">
+      <c r="I25" s="28">
+        <v>0</v>
+      </c>
+      <c r="J25" s="26">
+        <v>0</v>
+      </c>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="27">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="28">
+        <v>0</v>
+      </c>
+      <c r="R25" s="26">
+        <v>0</v>
+      </c>
+      <c r="S25" s="27">
         <v>0</v>
       </c>
     </row>
@@ -2182,26 +2238,26 @@
       </c>
       <c r="C26" s="24"/>
       <c r="D26" s="24"/>
-      <c r="I26" s="33">
-        <v>0</v>
-      </c>
-      <c r="J26" s="31">
-        <v>1</v>
-      </c>
-      <c r="K26" s="31"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="31"/>
-      <c r="N26" s="31"/>
-      <c r="O26" s="32">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="33">
-        <v>0</v>
-      </c>
-      <c r="R26" s="31">
-        <v>1</v>
-      </c>
-      <c r="S26" s="32">
+      <c r="I26" s="28">
+        <v>0</v>
+      </c>
+      <c r="J26" s="26">
+        <v>1</v>
+      </c>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="27">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="28">
+        <v>0</v>
+      </c>
+      <c r="R26" s="26">
+        <v>1</v>
+      </c>
+      <c r="S26" s="27">
         <v>1</v>
       </c>
     </row>
@@ -2209,26 +2265,26 @@
       <c r="B27" s="24"/>
       <c r="C27" s="24"/>
       <c r="D27" s="24"/>
-      <c r="I27" s="33">
-        <v>1</v>
-      </c>
-      <c r="J27" s="31">
-        <v>0</v>
-      </c>
-      <c r="K27" s="31"/>
-      <c r="L27" s="31"/>
-      <c r="M27" s="31"/>
-      <c r="N27" s="31"/>
-      <c r="O27" s="32">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="33">
-        <v>1</v>
-      </c>
-      <c r="R27" s="31">
-        <v>0</v>
-      </c>
-      <c r="S27" s="32">
+      <c r="I27" s="28">
+        <v>1</v>
+      </c>
+      <c r="J27" s="26">
+        <v>0</v>
+      </c>
+      <c r="K27" s="26"/>
+      <c r="L27" s="26"/>
+      <c r="M27" s="26"/>
+      <c r="N27" s="26"/>
+      <c r="O27" s="27">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="28">
+        <v>1</v>
+      </c>
+      <c r="R27" s="26">
+        <v>0</v>
+      </c>
+      <c r="S27" s="27">
         <v>1</v>
       </c>
     </row>
@@ -2238,26 +2294,26 @@
       </c>
       <c r="C28" s="24"/>
       <c r="D28" s="24"/>
-      <c r="I28" s="34">
-        <v>1</v>
-      </c>
-      <c r="J28" s="35">
-        <v>1</v>
-      </c>
-      <c r="K28" s="35"/>
-      <c r="L28" s="35"/>
-      <c r="M28" s="35"/>
-      <c r="N28" s="35"/>
-      <c r="O28" s="36">
-        <v>1</v>
-      </c>
-      <c r="Q28" s="34">
-        <v>1</v>
-      </c>
-      <c r="R28" s="35">
-        <v>1</v>
-      </c>
-      <c r="S28" s="36">
+      <c r="I28" s="29">
+        <v>1</v>
+      </c>
+      <c r="J28" s="30">
+        <v>1</v>
+      </c>
+      <c r="K28" s="30"/>
+      <c r="L28" s="30"/>
+      <c r="M28" s="30"/>
+      <c r="N28" s="30"/>
+      <c r="O28" s="31">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="29">
+        <v>1</v>
+      </c>
+      <c r="R28" s="30">
+        <v>1</v>
+      </c>
+      <c r="S28" s="31">
         <v>1</v>
       </c>
     </row>

</xml_diff>